<commit_message>
correct vocab mistake in n3 res file
</commit_message>
<xml_diff>
--- a/N3_Kanji.xlsx
+++ b/N3_Kanji.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProGramming_Projects\Python\KanjiBot\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProGramming_Projects\Python\KanjiBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0F9B3D-CCDB-48F6-A9A4-021038526582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF1D6CA-602A-49FC-9B89-66E140774748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,9 +463,6 @@
     <t>たまねぎ</t>
   </si>
   <si>
-    <t>Egg</t>
-  </si>
-  <si>
     <t>屋根</t>
   </si>
   <si>
@@ -560,6 +557,9 @@
   </si>
   <si>
     <t>Lost property</t>
+  </si>
+  <si>
+    <t>Onion</t>
   </si>
 </sst>
 </file>
@@ -822,8 +822,8 @@
   </sheetPr>
   <dimension ref="A1:C1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="51" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>146</v>
@@ -1398,120 +1398,120 @@
         <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>